<commit_message>
updated parser for non italic sensitivity
</commit_message>
<xml_diff>
--- a/Study/example_conditions.xlsx
+++ b/Study/example_conditions.xlsx
@@ -79,46 +79,46 @@
     <t>NextPathHeight</t>
   </si>
   <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorld.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\Student.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldInput.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentInput.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldRight.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentRight.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldWrong1.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentWrong1.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldWrong2.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentWrong2.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldDontKnow.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentDontKnow.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorldNext.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\StudentNext.png</t>
+    <t>..\CodeSnippets\Snippets\HelloWorld.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\Student.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldInput.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentInput.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldRight.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentRight.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldWrong1.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentWrong1.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldWrong2.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentWrong2.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldDontKnow.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentDontKnow.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\HelloWorldNext.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Snippets\StudentNext.png</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added parser and updated images
</commit_message>
<xml_diff>
--- a/Study/example_conditions.xlsx
+++ b/Study/example_conditions.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\NoviceVsExpert\Study\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3ACB65-CFE1-4DB8-8234-2D908529A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -85,6 +79,12 @@
     <t>NextPathHeight</t>
   </si>
   <si>
+    <t>..\CodeSnippets\Examples\Snippets\HelloWorld.png</t>
+  </si>
+  <si>
+    <t>..\CodeSnippets\Examples\Snippets\Student.png</t>
+  </si>
+  <si>
     <t>..\CodeSnippets\Examples\Snippets\HelloWorldInput.png</t>
   </si>
   <si>
@@ -119,19 +119,13 @@
   </si>
   <si>
     <t>..\CodeSnippets\Examples\Snippets\StudentNext.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\Student.png</t>
-  </si>
-  <si>
-    <t>..\CodeSnippets\Examples\Snippets\HelloWorld.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,23 +184,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -248,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,27 +266,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,24 +300,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,16 +475,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,9 +547,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>494</v>
@@ -610,7 +558,7 @@
         <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2">
         <v>494</v>
@@ -619,7 +567,7 @@
         <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>131</v>
@@ -628,7 +576,7 @@
         <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>65</v>
@@ -637,7 +585,7 @@
         <v>35</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="N2">
         <v>197</v>
@@ -646,7 +594,7 @@
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q2">
         <v>109</v>
@@ -655,7 +603,7 @@
         <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T2">
         <v>54</v>
@@ -664,9 +612,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>346</v>
@@ -675,7 +623,7 @@
         <v>352</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>402</v>
@@ -684,7 +632,7 @@
         <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>26</v>
@@ -693,7 +641,7 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K3">
         <v>26</v>
@@ -702,7 +650,7 @@
         <v>29</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N3">
         <v>50</v>
@@ -711,7 +659,7 @@
         <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q3">
         <v>34</v>
@@ -720,7 +668,7 @@
         <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T3">
         <v>42</v>

</xml_diff>